<commit_message>
Updated numbers for 2023.
</commit_message>
<xml_diff>
--- a/jack+jill.xlsx
+++ b/jack+jill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\harp.d\HARP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\ARP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BCFD42-74C5-4E90-9402-7EBC3DA00CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090096A0-B81E-4827-871A-719287C0FA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29520" yWindow="-6810" windowWidth="18285" windowHeight="15585" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -420,10 +420,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB57614-FCF1-4139-AA0D-31AF55A08D66}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B2" s="1">
         <v>100000</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B3" s="1">
         <v>100000</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B4" s="1">
         <v>100000</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -540,7 +540,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -553,7 +553,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -566,7 +566,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -579,7 +579,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -592,7 +592,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -605,7 +605,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -618,7 +618,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -631,7 +631,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -644,7 +644,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -657,7 +657,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -670,7 +670,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -683,7 +683,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -696,7 +696,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -709,7 +709,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -722,7 +722,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -735,7 +735,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -748,7 +748,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -761,7 +761,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -774,7 +774,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -787,7 +787,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -800,7 +800,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -813,7 +813,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -826,7 +826,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -839,7 +839,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -852,7 +852,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -865,7 +865,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -878,7 +878,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -889,19 +889,6 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>2054</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -910,10 +897,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DE7EE4-731B-47FB-9A4E-667972814602}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +947,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B2" s="1">
         <v>80000</v>
@@ -975,7 +962,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B3" s="1">
         <v>80000</v>
@@ -990,7 +977,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B4" s="1">
         <v>85000</v>
@@ -1005,7 +992,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1018,7 +1005,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1031,7 +1018,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1044,7 +1031,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1057,7 +1044,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1070,7 +1057,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1083,7 +1070,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1096,7 +1083,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1109,7 +1096,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1122,7 +1109,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1135,7 +1122,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1148,7 +1135,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1161,7 +1148,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1174,7 +1161,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1187,7 +1174,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1200,7 +1187,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1213,7 +1200,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1226,7 +1213,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1239,7 +1226,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1252,7 +1239,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1265,7 +1252,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1278,7 +1265,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1291,7 +1278,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1304,7 +1291,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1317,7 +1304,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1330,7 +1317,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1343,7 +1330,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1356,7 +1343,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1369,7 +1356,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1382,7 +1369,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1395,19 +1382,6 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2056</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36">
         <v>2057</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added name() function to Plan class for clarity.
</commit_message>
<xml_diff>
--- a/jack+jill.xlsx
+++ b/jack+jill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\ARP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090096A0-B81E-4827-871A-719287C0FA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577BA66F-595E-4C9F-B5F5-EA2FA1067F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -123,9 +123,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,7 +163,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -269,7 +269,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -411,7 +411,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,10 +420,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB57614-FCF1-4139-AA0D-31AF55A08D66}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,6 +889,11 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2055</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -897,10 +902,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DE7EE4-731B-47FB-9A4E-667972814602}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,6 +1390,11 @@
         <v>2057</v>
       </c>
     </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2058</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Clarified income -> wages in Excel file.
</commit_message>
<xml_diff>
--- a/jack+jill.xlsx
+++ b/jack+jill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\ARP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577BA66F-595E-4C9F-B5F5-EA2FA1067F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B774E32-F52B-471D-99CA-54EE4F61F0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>big ticket items</t>
   </si>
   <si>
-    <t>anticipated income</t>
-  </si>
-  <si>
     <t>Roth X</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>ctrb Roth IRA</t>
+  </si>
+  <si>
+    <t>anticipated wages</t>
   </si>
 </sst>
 </file>
@@ -422,57 +422,57 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -489,7 +489,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -506,7 +506,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -523,7 +523,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -538,7 +538,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -551,7 +551,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -564,7 +564,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -577,7 +577,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -590,7 +590,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -603,7 +603,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -616,7 +616,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -629,7 +629,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -642,7 +642,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -655,7 +655,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -668,7 +668,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -681,7 +681,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -694,7 +694,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -707,7 +707,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -720,7 +720,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -733,7 +733,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -746,7 +746,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -759,7 +759,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -772,7 +772,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -785,7 +785,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -798,7 +798,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -811,7 +811,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -837,7 +837,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2051</v>
       </c>
@@ -850,7 +850,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2052</v>
       </c>
@@ -863,7 +863,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2053</v>
       </c>
@@ -876,7 +876,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2054</v>
       </c>
@@ -889,7 +889,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2055</v>
       </c>
@@ -904,53 +904,53 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -980,7 +980,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -995,7 +995,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -1008,7 +1008,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -1021,7 +1021,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -1060,7 +1060,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -1073,7 +1073,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -1099,7 +1099,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -1125,7 +1125,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -1164,7 +1164,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -1177,7 +1177,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -1203,7 +1203,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -1229,7 +1229,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -1255,7 +1255,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -1281,7 +1281,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -1294,7 +1294,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -1307,7 +1307,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2051</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2052</v>
       </c>
@@ -1333,7 +1333,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2053</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2054</v>
       </c>
@@ -1359,7 +1359,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2055</v>
       </c>
@@ -1372,7 +1372,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2056</v>
       </c>
@@ -1385,12 +1385,12 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2057</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2058</v>
       </c>

</xml_diff>